<commit_message>
Finished revising my article
</commit_message>
<xml_diff>
--- a/Exam/Data/boxplot.xlsx
+++ b/Exam/Data/boxplot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Investigation-and-Reporting\Exam\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6075686B-CE85-4434-ABAE-89CB6F2E200A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5923156-AE98-405F-864B-AB1EA4C93C92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB91745A-5914-4BD8-BCD0-FDAAB81A943C}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -528,7 +528,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1497,8 +1497,8 @@
         <c:axId val="1877602575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.23500000000000001"/>
-          <c:min val="0.125"/>
+          <c:max val="0.22000000000000003"/>
+          <c:min val="0.12000000000000001"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1606,7 +1606,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2575,8 +2575,8 @@
         <c:axId val="2088346543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.10600000000000001"/>
-          <c:min val="9.600000000000003E-2"/>
+          <c:max val="0.19500000000000003"/>
+          <c:min val="9.5000000000000029E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2684,7 +2684,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3755,7 +3755,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6914,15 +6914,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>595312</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6950,15 +6950,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>576262</xdr:colOff>
+      <xdr:colOff>566737</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7095,7 +7095,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7393,8 +7393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0AF9E-F74B-450C-A4F7-C68CFBA16C6C}">
   <dimension ref="B3:M1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>